<commit_message>
10/26/2021 - added more UWI object data collection
</commit_message>
<xml_diff>
--- a/datacollection.xlsx
+++ b/datacollection.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,82 +440,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>100/08-12-066-25W5/00</t>
+          <t>100/03-36-065-25W5/00</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>102/07-12-066-25W5/00</t>
+          <t>100/07-36-065-25W5/00</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>102/02-12-066-25W5/00</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>100/07-36-065-25W5/00</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>102/10-36-065-25W5/00</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>100/03-36-065-25W5/00</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>102/13-06-068-24W5/00</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>103/13-06-068-24W5/00</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>102/14-06-068-24W5/00</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>100/14-06-068-24W5/00</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>103/14-06-068-24W5/00</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>100/16-01-068-25W5/00</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>100/08-01-068-25W5/00</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>100/01-18-068-24W5/00</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>100/09-01-068-25W5/00</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>100/16-14-068-25W5/00</t>
         </is>
       </c>
     </row>
@@ -526,52 +461,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>49</v>
+        <v>152</v>
       </c>
       <c r="C2" t="n">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D2" t="n">
-        <v>51</v>
-      </c>
-      <c r="E2" t="n">
-        <v>52</v>
-      </c>
-      <c r="F2" t="n">
         <v>106</v>
-      </c>
-      <c r="G2" t="n">
-        <v>152</v>
-      </c>
-      <c r="H2" t="n">
-        <v>118</v>
-      </c>
-      <c r="I2" t="n">
-        <v>93</v>
-      </c>
-      <c r="J2" t="n">
-        <v>79</v>
-      </c>
-      <c r="K2" t="n">
-        <v>87</v>
-      </c>
-      <c r="L2" t="n">
-        <v>107</v>
-      </c>
-      <c r="M2" t="n">
-        <v>89</v>
-      </c>
-      <c r="N2" t="n">
-        <v>109</v>
-      </c>
-      <c r="O2" t="n">
-        <v>77</v>
-      </c>
-      <c r="P2" t="n">
-        <v>113</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>136</v>
       </c>
     </row>
     <row r="3">
@@ -581,52 +477,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>141</v>
+        <v>419</v>
       </c>
       <c r="C3" t="n">
-        <v>81</v>
+        <v>239</v>
       </c>
       <c r="D3" t="n">
-        <v>183</v>
-      </c>
-      <c r="E3" t="n">
-        <v>238</v>
-      </c>
-      <c r="F3" t="n">
-        <v>372</v>
-      </c>
-      <c r="G3" t="n">
-        <v>418</v>
-      </c>
-      <c r="H3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I3" t="n">
-        <v>63</v>
-      </c>
-      <c r="J3" t="n">
-        <v>280</v>
-      </c>
-      <c r="K3" t="n">
-        <v>241</v>
-      </c>
-      <c r="L3" t="n">
-        <v>178</v>
-      </c>
-      <c r="M3" t="n">
-        <v>138</v>
-      </c>
-      <c r="N3" t="n">
-        <v>41</v>
-      </c>
-      <c r="O3" t="n">
-        <v>41</v>
-      </c>
-      <c r="P3" t="n">
-        <v>41</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>25</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4">
@@ -636,52 +493,29 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44353.47916666666</v>
+        <v>44076.33333333334</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44413.625</v>
+        <v>44256.29166666666</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44311.54166666666</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>44256.29166666666</v>
-      </c>
-      <c r="F4" s="2" t="n">
         <v>44122.41666666666</v>
       </c>
-      <c r="G4" s="2" t="n">
-        <v>44076.33333333334</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>44488.3125</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>44431.4375</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>44214.58333333334</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>44253.29166666666</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>44316.29166666666</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>44356.29166666666</v>
-      </c>
-      <c r="N4" s="2" t="n">
-        <v>44453.60416666666</v>
-      </c>
-      <c r="O4" s="2" t="n">
-        <v>44453.54166666666</v>
-      </c>
-      <c r="P4" s="2" t="n">
-        <v>44453.5</v>
-      </c>
-      <c r="Q4" s="2" t="n">
-        <v>44469.52083333334</v>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Num of WS Jobs</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>22</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021/10/26 Logic (but not error catching) built
</commit_message>
<xml_diff>
--- a/datacollection.xlsx
+++ b/datacollection.xlsx
@@ -445,12 +445,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>102/10-36-065-25W5/00</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>100/07-36-065-25W5/00</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>102/10-36-065-25W5/00</t>
         </is>
       </c>
     </row>
@@ -464,10 +464,10 @@
         <v>152</v>
       </c>
       <c r="C2" t="n">
+        <v>106</v>
+      </c>
+      <c r="D2" t="n">
         <v>52</v>
-      </c>
-      <c r="D2" t="n">
-        <v>106</v>
       </c>
     </row>
     <row r="3">
@@ -480,10 +480,10 @@
         <v>419</v>
       </c>
       <c r="C3" t="n">
+        <v>373</v>
+      </c>
+      <c r="D3" t="n">
         <v>239</v>
-      </c>
-      <c r="D3" t="n">
-        <v>373</v>
       </c>
     </row>
     <row r="4">
@@ -496,10 +496,10 @@
         <v>44076.33333333334</v>
       </c>
       <c r="C4" s="2" t="n">
+        <v>44122.41666666666</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>44256.29166666666</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>44122.41666666666</v>
       </c>
     </row>
     <row r="5">
@@ -512,10 +512,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
         <v>22</v>
-      </c>
-      <c r="D5" t="n">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>